<commit_message>
Simaple Demo & init 2024/02/27
</commit_message>
<xml_diff>
--- a/Resources/DataFiles/TestData_Dev.xlsx
+++ b/Resources/DataFiles/TestData_Dev.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27304"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PycharmProject\ExcelExcuteTestFromework\Resources\DateFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PycharmProject\ExcelExcuteTestFromework\Resources\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2B4488-3C1C-45BC-9845-332FE9B3B746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128854FB-98AC-4302-A358-68C665755E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21624" yWindow="804" windowWidth="14160" windowHeight="12120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="3648" windowWidth="16596" windowHeight="12912" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add" sheetId="1" r:id="rId1"/>
-    <sheet name="baidu" sheetId="2" r:id="rId2"/>
+    <sheet name="baidu" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>status</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -70,6 +70,9 @@
   <si>
     <t>Tesitng</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normal</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection activeCell="D13" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -515,67 +518,60 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC2D916C-B0EC-4EE9-BFBB-963C728EEFDC}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D27CD8B4-13A9-4FC9-A3FC-99D657CDE750}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D7" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>